<commit_message>
Updated the rejection notification script to send to members of a group.
</commit_message>
<xml_diff>
--- a/ContentHub.MockImplementation/import/mock_data.xlsx
+++ b/ContentHub.MockImplementation/import/mock_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasfomic\Desktop\Content Hub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vasfomic\Desktop\mock-implementation\ContentHub.MockImplementation\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,14 +22,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="124">
   <si>
     <t>File</t>
   </si>
   <si>
-    <t>https://sldemoassets.blob.core.windows.net/sldemoassets/dam-pro-final/alexander-mils-667996.jpg</t>
-  </si>
-  <si>
     <t>https://sldemoassets.blob.core.windows.net/sldemoassets/dam-pro-final/arno-smit-141735.jpg</t>
   </si>
   <si>
@@ -391,6 +388,12 @@
   </si>
   <si>
     <t>FinalLifeCycleStatusToAsset</t>
+  </si>
+  <si>
+    <t>https://www.lexus.com/-/media/TMNA.LEXC/Project/Lexus/Homepage/Shopping-Tools/icons/Lexus-byl-homepage-shopping-tool_80x23.jpg?rev=d5eddeecc58644ddbe13ab631b6d6f61&amp;h=23&amp;w=80&amp;la=en&amp;hash=7013F1B9D3C08C3FEEF03EB223D3D5F7</t>
+  </si>
+  <si>
+    <t>Created</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45"/>
@@ -781,2129 +784,2129 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
         <v>117</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" t="s">
         <v>121</v>
-      </c>
-      <c r="E1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.6">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.6">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.6">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.6">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.6">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.6">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.6">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.6">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.6">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.6">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.6">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.6">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.6">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.6">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="s">
         <v>102</v>
       </c>
-      <c r="G15" t="s">
-        <v>103</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.6">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.6">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.6">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.6">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" t="s">
         <v>102</v>
       </c>
-      <c r="G19" t="s">
-        <v>103</v>
-      </c>
       <c r="H19" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.6">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.6">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.6">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.6">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.6">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.6">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.6">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.6">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.6">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.6">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.6">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.6">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.6">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.6">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="14.6">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.6">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F35" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G35" t="s">
         <v>102</v>
       </c>
-      <c r="G35" t="s">
-        <v>103</v>
-      </c>
       <c r="H35" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.6">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.6">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.6">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.6">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F39" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G39" t="s">
         <v>102</v>
       </c>
-      <c r="G39" t="s">
-        <v>103</v>
-      </c>
       <c r="H39" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.6">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.6">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="14.6">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.6">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14.6">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.6">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="14.6">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.6">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="14.6">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.6">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.6">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.6">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C51" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.6">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.6">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.6">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="14.6">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="14.6">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="14.6">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="14.6">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="14.6">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="14.6">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D60" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="14.6">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G61" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="14.6">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="14.6">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C63" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="14.6">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C64" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="14.6">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G65" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="14.6">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="14.6">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="14.6">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C68" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="14.6">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C69" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="14.6">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="14.6">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D71" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F71" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G71" t="s">
         <v>102</v>
       </c>
-      <c r="G71" t="s">
-        <v>103</v>
-      </c>
       <c r="H71" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="14.6">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C72" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="14.6">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C73" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D73" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="14.6">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D74" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G74" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="14.6">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G75" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="14.6">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="14.6">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="14.6">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="14.6">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F79" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G79" t="s">
         <v>102</v>
       </c>
-      <c r="G79" t="s">
-        <v>103</v>
-      </c>
       <c r="H79" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="14.6">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C80" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D80" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E80" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="14.6">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="14.6">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C82" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D82" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E82" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G82" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="14.6">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C83" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D83" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F83" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G83" t="s">
         <v>102</v>
       </c>
-      <c r="G83" t="s">
-        <v>103</v>
-      </c>
       <c r="H83" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="14.6">
       <c r="A84" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C84" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D84" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E84" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="14.6">
       <c r="A85" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
+        <v>110</v>
+      </c>
+      <c r="C85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D85" t="s">
+        <v>91</v>
+      </c>
+      <c r="E85" t="s">
         <v>111</v>
       </c>
-      <c r="C85" t="s">
-        <v>111</v>
-      </c>
-      <c r="D85" t="s">
-        <v>92</v>
-      </c>
-      <c r="E85" t="s">
-        <v>112</v>
-      </c>
       <c r="F85" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="14.6">
       <c r="A86" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C86" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="14.6">
       <c r="A87" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D87" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E87" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G87" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="14.6">
       <c r="A88" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C88" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E88" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="G88" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="14.6">
       <c r="A89" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C89" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G89" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="14.6">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G90" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="14.6">

</xml_diff>